<commit_message>
Update to send stickers
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>Meme</t>
   </si>
@@ -19,30 +19,45 @@
     <t>URL</t>
   </si>
   <si>
+    <t>StickerID</t>
+  </si>
+  <si>
     <t>en fin la hipocresia</t>
   </si>
   <si>
     <t>https://plantillasdememes.com/img/plantillas/en-fin-la-hipocresia01590648604.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPlmAJgWeGgC56x_QlfmkfGA6u1-EXAAJkAAPFhdoNqWIhAoi3HgweBA</t>
+  </si>
+  <si>
     <t>es mi don mi maldicion</t>
   </si>
   <si>
     <t>https://plantillasdememes.com/img/plantillas/este-es-mi-don-mi-maldicion31608160957.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPmmAJga6Km-7KpfMqZFfdCSIUMq2wAAJmAAPFhdoN2S5P0NzcZdkeBA</t>
+  </si>
+  <si>
     <t>se tenia que decir y se dijo</t>
   </si>
   <si>
     <t>https://plantillasdememes.com/img/plantillas/se-tenia-que-decir-y-se-dijo4.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPmGAJgZvUXiHx1njgcyv96Lcr7pJGAAJlAAPFhdoNhYeqltSpqnEeBA</t>
+  </si>
+  <si>
     <t>puta que oferton</t>
   </si>
   <si>
     <t>https://plantillasdememes.com/img/plantillas/puta-que-oferton5.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPnGAJgbs7PX33F0Y9jALNwpXzZMQoAAJoAAPFhdoNoMvJboxbdSIeBA</t>
+  </si>
+  <si>
     <t>chupalo</t>
   </si>
   <si>
@@ -61,22 +76,34 @@
     <t>https://www.generadormemes.com/media/created/1200x675xjnhrib.jpg.pagespeed.ic.meme.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPomAJgfNvkQwakOn_NA3gBsOdYfNHAAJqAAPFhdoNqadhusjy-toeBA</t>
+  </si>
+  <si>
     <t>hay</t>
   </si>
   <si>
     <t>https://i.pinimg.com/236x/c6/18/d4/c618d4932f424a4ebe06b0145c902ae4.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPpGAJggVYD5UWVNCQXz-Wu7jNFdNPAAJrAAPFhdoNAAG6b0TkGD33HgQ</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
     <t>https://i.pinimg.com/originals/df/77/df/df77df41a66ab81f6143a943f5979295.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPpmAJghMkDN2tmlgUwd1tda7cofV5AAJsAAPFhdoNmnoCWGJwQtgeBA</t>
+  </si>
+  <si>
     <t>dorime</t>
   </si>
   <si>
     <t>https://elcomercio.pe/resizer/1Kuka3Nhcm8wRVmFeHsDdH1DG4U=/1200x1200/smart/filters:format(jpeg):quality(75)/dvgnzpfv30f28.cloudfront.net/12-18-2019/t_7020f15221224dd4be7cec5cfa9d887e_name_dorime_1.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIPqGAJghz4UuY_9F8z8uUw6YaFnILXAAJtAAPFhdoN2LBUflEyZ-QeBA</t>
   </si>
   <si>
     <t>ya estoy harto</t>
@@ -90,11 +117,18 @@
       <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTo8Om7uf9vjw3dfdynHWbyOnyVFzngQWPZmg&amp;usqp=CA</t>
     </r>
     <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPqmAJgig49B1cBrWIY4VvCXBVLhdBAAJuAAPFhdoNgaNuTCq8S6EeBA</t>
+  </si>
+  <si>
     <t>ya estoy harta</t>
   </si>
   <si>
@@ -107,30 +141,45 @@
     <t>https://static.wixstatic.com/media/16fbb1_5e5fc96a51f64684bd83069e9df418a1~mv2.png/v1/fill/w_700,h_700,al_c/icon.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPrGAJgjQ9Uf2khdWOgkO9p8dx_0_hAAJvAAPFhdoNf5vXQNR_yhceBA</t>
+  </si>
+  <si>
     <t>habla pues</t>
   </si>
   <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQM8TwIQa5z7igmWelwBAltRlz83Asd2fRuoA&amp;usqp=CAU</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPrmAJgkGYuimOObTBY52rguQF0lirAAJwAAPFhdoNupZSmgjwQQgeBA</t>
+  </si>
+  <si>
     <t>duren</t>
   </si>
   <si>
     <t>https://i.pinimg.com/originals/c9/14/69/c91469743709baa3f3a9acc72b2a7bac.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPsGAJglWdM9-UHMPhiq0giepp6GchAAJxAAPFhdoNDlnkuRvA9aUeBA</t>
+  </si>
+  <si>
     <t>tenemos</t>
   </si>
   <si>
     <t>https://www.cinepremiere.com.mx/wp-content/uploads/2020/06/Bugs-Bunny-1024x559.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPsmAJgl6-qVbAdULXOxau8-b_Ei7hAAJyAAPFhdoNvP31XUNUpt4eBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">tas bien </t>
   </si>
   <si>
     <t>https://i.pinimg.com/originals/98/6f/36/986f36b6919c1817f70fd0ab707c1ac6.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPtGAJgmgY8u_nnOZqX-oFRr3HNfuuAAJzAAPFhdoNbUukgr_b_2MeBA</t>
+  </si>
+  <si>
     <t>estás bien</t>
   </si>
   <si>
@@ -140,12 +189,18 @@
     <t>https://i.pinimg.com/736x/4d/88/e4/4d88e4c31d839f33eb837a556e30696e.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPtmAJgnXFGcOUxOT1RSlfyjktEMRtAAJ0AAPFhdoNfKcqsiXSkPceBA</t>
+  </si>
+  <si>
     <t>porfa</t>
   </si>
   <si>
     <t>https://www.generadormemes.com/media/templates/gato_de_shrek.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPuGAJgnzVv0G3t2UCiHt3g2mrBfZ5AAJ1AAPFhdoNubPy3epbSqUeBA</t>
+  </si>
+  <si>
     <t>por favor</t>
   </si>
   <si>
@@ -155,12 +210,18 @@
     <t>https://i.ytimg.com/vi/TunKOUfUNYw/maxresdefault.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPumAJgoXe-0DML9n5_QuBBX32cnyyAAJ2AAPFhdoN8albyG4HsLweBA</t>
+  </si>
+  <si>
     <t>Que ?</t>
   </si>
   <si>
     <t>https://pbs.twimg.com/media/EZYbhsmXkAABI5s.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPvGAJgo82HNwrb6zz89mvX2Q-M1XmAAJ3AAPFhdoN89zVLnuvkwUeBA</t>
+  </si>
+  <si>
     <t>khe ?</t>
   </si>
   <si>
@@ -176,6 +237,9 @@
     <t>https://gluc.mx/u/fotografias/m/2020/6/17/f850x638-28837_106326_5050.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPvmAJgp1PbtEDuxVX3_OO_aZ0nFrHAAJ4AAPFhdoNBBFlw8oIoXUeBA</t>
+  </si>
+  <si>
     <t>a dormir</t>
   </si>
   <si>
@@ -191,36 +255,54 @@
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRW3rrOYu6-9w6tC7uaVIYnPflkjuk5OSyt3w&amp;usqp=CAU</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPwGAJgr-42wMFYYrDKP5HfYsh_l8LAAJ5AAPFhdoNyGqGj27rAAEOHgQ</t>
+  </si>
+  <si>
     <t>callate</t>
   </si>
   <si>
     <t>https://img.buzzfeed.com/buzzfeed-static/static/2018-05/18/11/campaign_images/buzzfeed-prod-web-01/si-haces-45-de-estas-60-cosas-tenemos-que-decirte-2-17831-1526658218-4_dblbig.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPwmAJgsfvjNRQBxwwDHB4STO96gbdAAJ6AAPFhdoNr9xppgTXM14eBA</t>
+  </si>
+  <si>
     <t>para mas placer</t>
   </si>
   <si>
     <t>https://64.media.tumblr.com/f1e8538cb67140b26cb8ae3705dd6cfa/tumblr_ngg8gnIJaj1tszwcio1_1280.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPxGAJgs-ngetxXnaBZYOor_MyevR_AAJ7AAPFhdoNzG-tl214NzIeBA</t>
+  </si>
+  <si>
     <t>si si ya a la chingada</t>
   </si>
   <si>
     <t>https://plantillasdememes.com/img/plantillas/si-si-ya-ala-chingada51580498748.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPxmAJgtiMCJvplYnRXIROJ-81RCU8AAJ8AAPFhdoNYEjnFsDxL4EeBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">y ahora </t>
   </si>
   <si>
     <t>https://i.imgflip.com/31e94y.png</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPyGAJgvKEP9Z_YbTJx63Gj6uvnXJCAAJ9AAPFhdoNLmg3_4VAjKEeBA</t>
+  </si>
+  <si>
     <t>por que me persigue la desgracia</t>
   </si>
   <si>
     <t>https://i.postimg.cc/XvhbQrW8/lossimpson-60635f75c23d0cd12017cb8129f30b1b-1200x800.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPymAJgvq3_tFCfEz88Z7Stq_vXiXQAAJ-AAPFhdoNf3PtAYKuPpMeBA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Por que nos persigue la desgracia </t>
   </si>
   <si>
@@ -230,58 +312,169 @@
     <t>https://postimg.cc/hf693Lpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPzGAJgwOxi_O27CZ0gjAUpfdsyWuMAAJ_AAPFhdoN9qQLkJcV1S4eBA</t>
+  </si>
+  <si>
     <t>es un hechizo simple pero inquebrantable</t>
   </si>
   <si>
     <t>https://i.postimg.cc/13w5gcZQ/es-un-hechizo-simple-pero-inquebrantable2-2.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIPzmAJgw2sDch1x8xjE9Pv_l1a8h9KAAKAAAPFhdoNdy7e_-kRnfUeBA</t>
+  </si>
+  <si>
     <t>y volo</t>
   </si>
   <si>
     <t>https://cdn.memegenerator.es/imagenes/memes/thumb/26/28/26280808.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP0GAJgxXh-m8ybuLMcrwElCOmZpHkAAKBAAPFhdoNyWBkc49M6gYeBA</t>
+  </si>
+  <si>
     <t>si bueno quien tiene hambre</t>
   </si>
   <si>
     <t>https://i.postimg.cc/505py01P/si-bueno-quien-tiene-hambre11564186254.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP0mAJgx6fXuTPi_JI4tCumFXQkvdDAAKCAAPFhdoNXZeTHF9mW8EeBA</t>
+  </si>
+  <si>
     <t>no lo se tu dime</t>
   </si>
   <si>
     <t>https://i.postimg.cc/1XwgsnQt/no-lo-se-tu-dime4.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP1GAJgyhLxOx916LSY-BniUj0DBj4AAKDAAPFhdoND9rJVyGNLM0eBA</t>
+  </si>
+  <si>
     <t>wey ya</t>
   </si>
   <si>
     <t>https://i.postimg.cc/cJwP7d03/wey-ya31580921271.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP1mAJgzO5IIBa6_QDQE1IDgABgIkbiwAChAADxYXaDU0y_plCEhXYHgQ</t>
+  </si>
+  <si>
     <t>ah caray eso si me interesa</t>
   </si>
   <si>
     <t>https://i.postimg.cc/j5Xd2Nj3/ah-caray-eso-si-me-interesa2.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP2GAJg0GjxmOhTM3-yuPU1RvvrA3PAAKFAAPFhdoNUu7xJ0GHofMeBA</t>
+  </si>
+  <si>
     <t>ya nos exhibiste</t>
   </si>
   <si>
     <t>https://i.postimg.cc/fRz4WFds/ya-nos-exhibiste2.jpg</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP2mAJg0m1u53r-uTW3Gg4ltAhXzcMAAKGAAPFhdoNxyAfdDnyzmQeBA</t>
+  </si>
+  <si>
     <t>lo logro</t>
   </si>
   <si>
     <t>https://www.memegenerator.es/meme/31165286</t>
   </si>
   <si>
+    <t>CAACAgEAAxkBAAIP3GAJg1PGsEbbYmJhC-DSeEw2vn2cAAKHAAPFhdoNNux324d3BfoeBA</t>
+  </si>
+  <si>
     <t>ve cerdo miserable</t>
   </si>
   <si>
     <t>https://i.postimg.cc/0yVKntZw/photo-2021-01-14-20-18-09.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP3mAJg1tAkNO2-xhhezOnsY-FsUUsAAKIAAPFhdoNl2XIa_dOkgseBA</t>
+  </si>
+  <si>
+    <t>absolutely subarashi</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/BZwqmrGs/subarashi.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP4GAJg2U6zMSxKkvqKNxUxQWQWGA1AAKJAAPFhdoNHdV_Szyf8xAeBA</t>
+  </si>
+  <si>
+    <t>pasa algo?</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/25GnBkLn/STK-20190220-WA0017.png</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP4mAJg24kJIE6msK7TzfQ-RoAAXD5RQACigADxYXaDS4sA8SYOFOPHgQ</t>
+  </si>
+  <si>
+    <t>ya me puse la pijama</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/dV42SRwz/STK-20190425-WA0024.png</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP5GAJg3ZhsU5N2iXpJJME7x7k-7FwAAKLAAPFhdoN21IycCeCvQoeBA</t>
+  </si>
+  <si>
+    <t>q se armen</t>
+  </si>
+  <si>
+    <t>https://postimg.cc/JtY6zd86</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP5mAJg4HJPWdX9wAB3087HI8HLx6IpAACjAADxYXaDXv3m4GkcYWPHgQ</t>
+  </si>
+  <si>
+    <t>no me digas que hacer</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/y6p4Bs9j/24883568-152148462076571-539314063090420184-o.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP6GAJg4q7rzXtOgs2MnbWNQO4hTXAAAKNAAPFhdoNT6jqwZbOcWMeBA</t>
+  </si>
+  <si>
+    <t>te creo pero mi metralleta no</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/wj6GsrhM/69549469-409057799718968-5926320364647874560-o.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP6mAJg5KNkAtuwbtyyRa6_zXTCSGsAAKOAAPFhdoNPvllKSUlSvgeBA</t>
+  </si>
+  <si>
+    <t>por que lo dice tan brusco</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/BnYMPnS7/Es-DSXNDVQAASFOH.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP7GAJg5rkMMbHFxePn1hsYdc8fYTtAAKPAAPFhdoN5B0TmaB0bDceBA</t>
+  </si>
+  <si>
+    <t>que trucazo no</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/FHRxvXyy/Er-f-Y5v-WMAIju4.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP7mAJg6bRAV94W8vgGLwAAUAvFTvW4wACkAADxYXaDVgSGTLYexBaHgQ</t>
+  </si>
+  <si>
+    <t>chucha ya</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/q7P3NbSL/url.jpg</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIP8GAJg61GasvgmSif0j2w2j3mEGlKAAKRAAPFhdoNDvNeBScVwNoeBA</t>
   </si>
 </sst>
 </file>
@@ -298,16 +491,17 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF1155CC"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -570,381 +764,624 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" ht="18.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>45</v>
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>3</v>
+        <v>73</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
+      <c r="A32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>57</v>
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>59</v>
+      <c r="A34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>60</v>
+      <c r="A35" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>61</v>
+        <v>84</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>63</v>
+      <c r="A36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="s">
-        <v>64</v>
+      <c r="A37" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>66</v>
+      <c r="A38" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>65</v>
+        <v>90</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>93</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>70</v>
+        <v>96</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>72</v>
+        <v>99</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>78</v>
+        <v>109</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>80</v>
+        <v>111</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>115</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>84</v>
+        <v>117</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +1433,16 @@
     <hyperlink r:id="rId45" ref="B46"/>
     <hyperlink r:id="rId46" ref="B47"/>
     <hyperlink r:id="rId47" ref="B48"/>
+    <hyperlink r:id="rId48" ref="B49"/>
+    <hyperlink r:id="rId49" ref="B50"/>
+    <hyperlink r:id="rId50" ref="B51"/>
+    <hyperlink r:id="rId51" ref="B52"/>
+    <hyperlink r:id="rId52" ref="B53"/>
+    <hyperlink r:id="rId53" ref="B54"/>
+    <hyperlink r:id="rId54" ref="B55"/>
+    <hyperlink r:id="rId55" ref="B56"/>
+    <hyperlink r:id="rId56" ref="B57"/>
   </hyperlinks>
-  <drawing r:id="rId48"/>
+  <drawing r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted function to get urls also deleted from excel
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,78 +11,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="283">
   <si>
     <t>Meme</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>StickerID</t>
   </si>
   <si>
     <t>en fin la hipocresia | en fin</t>
   </si>
   <si>
-    <t>https://plantillasdememes.com/img/plantillas/en-fin-la-hipocresia01590648604.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPlmAJgWeGgC56x_QlfmkfGA6u1-EXAAJkAAPFhdoNqWIhAoi3HgweBA</t>
   </si>
   <si>
     <t>es mi don mi maldicion</t>
   </si>
   <si>
-    <t>https://plantillasdememes.com/img/plantillas/este-es-mi-don-mi-maldicion31608160957.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPmmAJga6Km-7KpfMqZFfdCSIUMq2wAAJmAAPFhdoN2S5P0NzcZdkeBA</t>
   </si>
   <si>
+    <t>que ? | khe ? | khe | que | que?</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIdEGAqEeKS6rPVNRuB2WDKGmup7-gWAAJ3AAPFhdoN89zVLnuvkwUeBA</t>
+  </si>
+  <si>
     <t>se tenia que decir y se dijo</t>
   </si>
   <si>
-    <t>https://plantillasdememes.com/img/plantillas/se-tenia-que-decir-y-se-dijo4.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPmGAJgZvUXiHx1njgcyv96Lcr7pJGAAJlAAPFhdoNhYeqltSpqnEeBA</t>
   </si>
   <si>
     <t>puta que oferton</t>
   </si>
   <si>
-    <t>https://plantillasdememes.com/img/plantillas/puta-que-oferton5.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPnGAJgbs7PX33F0Y9jALNwpXzZMQoAAJoAAPFhdoNoMvJboxbdSIeBA</t>
   </si>
   <si>
     <t>chupalo</t>
   </si>
   <si>
-    <t>https://media.makeameme.org/created/chupalo-5b7ef3.jpg</t>
-  </si>
-  <si>
-    <t>No puede ser</t>
-  </si>
-  <si>
-    <t>https://i.pinimg.com/236x/a5/e9/48/a5e94838ef00cc4a891929f8104271f7.jpg</t>
+    <t>CAACAgEAAxkBAAIbsmAp3jwXwIUGRxMw6uJDW6lvoNHzAAJnAAPFhdoNgFdzAypF_8oeBA</t>
+  </si>
+  <si>
+    <t>no puede ser</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIbwGAp3yqz-_zYulzwwiPMDP_DLijrAAJpAAPFhdoNWMd92cV6AYgeBA</t>
   </si>
   <si>
     <t>andate a la verga</t>
   </si>
   <si>
-    <t>https://www.generadormemes.com/media/created/1200x675xjnhrib.jpg.pagespeed.ic.meme.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPomAJgfNvkQwakOn_NA3gBsOdYfNHAAJqAAPFhdoNqadhusjy-toeBA</t>
   </si>
   <si>
-    <t>hay</t>
-  </si>
-  <si>
-    <t>https://i.pinimg.com/236x/c6/18/d4/c618d4932f424a4ebe06b0145c902ae4.jpg</t>
+    <t>hay | ay</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPpGAJggVYD5UWVNCQXz-Wu7jNFdNPAAJrAAPFhdoNAAG6b0TkGD33HgQ</t>
@@ -91,57 +76,28 @@
     <t>no</t>
   </si>
   <si>
-    <t>https://i.pinimg.com/originals/df/77/df/df77df41a66ab81f6143a943f5979295.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPpmAJghMkDN2tmlgUwd1tda7cofV5AAJsAAPFhdoNmnoCWGJwQtgeBA</t>
   </si>
   <si>
     <t>dorime</t>
   </si>
   <si>
-    <t>https://elcomercio.pe/resizer/1Kuka3Nhcm8wRVmFeHsDdH1DG4U=/1200x1200/smart/filters:format(jpeg):quality(75)/dvgnzpfv30f28.cloudfront.net/12-18-2019/t_7020f15221224dd4be7cec5cfa9d887e_name_dorime_1.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPqGAJghz4UuY_9F8z8uUw6YaFnILXAAJtAAPFhdoN2LBUflEyZ-QeBA</t>
   </si>
   <si>
     <t>ya estoy harto | ya estoy harta</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTo8Om7uf9vjw3dfdynHWbyOnyVFzngQWPZmg&amp;usqp=CA</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPqmAJgig49B1cBrWIY4VvCXBVLhdBAAJuAAPFhdoNgaNuTCq8S6EeBA</t>
   </si>
   <si>
     <t>ayuda</t>
   </si>
   <si>
-    <t>https://static.wixstatic.com/media/16fbb1_5e5fc96a51f64684bd83069e9df418a1~mv2.png/v1/fill/w_700,h_700,al_c/icon.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPrGAJgjQ9Uf2khdWOgkO9p8dx_0_hAAJvAAPFhdoNf5vXQNR_yhceBA</t>
   </si>
   <si>
-    <t>habla pues</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQM8TwIQa5z7igmWelwBAltRlz83Asd2fRuoA&amp;usqp=CAU</t>
+    <t>habla pues | llora pues</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPrmAJgkGYuimOObTBY52rguQF0lirAAJwAAPFhdoNupZSmgjwQQgeBA</t>
@@ -150,91 +106,52 @@
     <t>duren</t>
   </si>
   <si>
-    <t>https://i.pinimg.com/originals/c9/14/69/c91469743709baa3f3a9acc72b2a7bac.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPsGAJglWdM9-UHMPhiq0giepp6GchAAJxAAPFhdoNDlnkuRvA9aUeBA</t>
   </si>
   <si>
     <t>tenemos</t>
   </si>
   <si>
-    <t>https://www.cinepremiere.com.mx/wp-content/uploads/2020/06/Bugs-Bunny-1024x559.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPsmAJgl6-qVbAdULXOxau8-b_Ei7hAAJyAAPFhdoNvP31XUNUpt4eBA</t>
   </si>
   <si>
     <t>tas bien | estas bien</t>
   </si>
   <si>
-    <t>https://i.pinimg.com/originals/98/6f/36/986f36b6919c1817f70fd0ab707c1ac6.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPtGAJgmgY8u_nnOZqX-oFRr3HNfuuAAJzAAPFhdoNbUukgr_b_2MeBA</t>
   </si>
   <si>
     <t>uy</t>
   </si>
   <si>
-    <t>https://i.pinimg.com/736x/4d/88/e4/4d88e4c31d839f33eb837a556e30696e.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPtmAJgnXFGcOUxOT1RSlfyjktEMRtAAJ0AAPFhdoNfKcqsiXSkPceBA</t>
   </si>
   <si>
-    <t>porfa</t>
-  </si>
-  <si>
-    <t>https://www.generadormemes.com/media/templates/gato_de_shrek.jpg</t>
+    <t>porfa | por favor</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPuGAJgnzVv0G3t2UCiHt3g2mrBfZ5AAJ1AAPFhdoNubPy3epbSqUeBA</t>
   </si>
   <si>
-    <t>por favor</t>
-  </si>
-  <si>
     <t>verga</t>
   </si>
   <si>
-    <t>https://i.ytimg.com/vi/TunKOUfUNYw/maxresdefault.jpg</t>
-  </si>
-  <si>
-    <t>CAACAgEAAxkBAAIPumAJgoXe-0DML9n5_QuBBX32cnyyAAJ2AAPFhdoN8albyG4HsLweBA</t>
-  </si>
-  <si>
-    <t>Que ? | khe ? | khe | que</t>
-  </si>
-  <si>
-    <t>https://pbs.twimg.com/media/EZYbhsmXkAABI5s.jpg</t>
-  </si>
-  <si>
-    <t>CAACAgEAAxkBAAIPvGAJgo82HNwrb6zz89mvX2Q-M1XmAAJ3AAPFhdoN89zVLnuvkwUeBA</t>
+    <t>CAACAgEAAxkBAAIb9GAp8kP5UyaIoD18vAAB7K2HAAG7ugADdgADxYXaDfGpW8huB7C8HgQ</t>
   </si>
   <si>
     <t>a mimir | a dormir | me voy a dormir</t>
   </si>
   <si>
-    <t>https://gluc.mx/u/fotografias/m/2020/6/17/f850x638-28837_106326_5050.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPvmAJgp1PbtEDuxVX3_OO_aZ0nFrHAAJ4AAPFhdoNBBFlw8oIoXUeBA</t>
   </si>
   <si>
-    <t>ya sientese</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRW3rrOYu6-9w6tC7uaVIYnPflkjuk5OSyt3w&amp;usqp=CAU</t>
+    <t>ya sientese | ya callese</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPwGAJgr-42wMFYYrDKP5HfYsh_l8LAAJ5AAPFhdoNyGqGj27rAAEOHgQ</t>
   </si>
   <si>
-    <t>callate</t>
-  </si>
-  <si>
-    <t>https://img.buzzfeed.com/buzzfeed-static/static/2018-05/18/11/campaign_images/buzzfeed-prod-web-01/si-haces-45-de-estas-60-cosas-tenemos-que-decirte-2-17831-1526658218-4_dblbig.jpg</t>
+    <t>callate | el huevo</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPwmAJgsfvjNRQBxwwDHB4STO96gbdAAJ6AAPFhdoNr9xppgTXM14eBA</t>
@@ -243,16 +160,10 @@
     <t>para mas placer</t>
   </si>
   <si>
-    <t>https://64.media.tumblr.com/f1e8538cb67140b26cb8ae3705dd6cfa/tumblr_ngg8gnIJaj1tszwcio1_1280.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPxGAJgs-ngetxXnaBZYOor_MyevR_AAJ7AAPFhdoNzG-tl214NzIeBA</t>
   </si>
   <si>
-    <t>si si ya a la chingada</t>
-  </si>
-  <si>
-    <t>https://plantillasdememes.com/img/plantillas/si-si-ya-ala-chingada51580498748.png</t>
+    <t>si si ya a la chingada | ya a la chingada | a la chingada</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPxmAJgtiMCJvplYnRXIROJ-81RCU8AAJ8AAPFhdoNYEjnFsDxL4EeBA</t>
@@ -261,25 +172,16 @@
     <t xml:space="preserve">y ahora </t>
   </si>
   <si>
-    <t>https://i.imgflip.com/31e94y.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPyGAJgvKEP9Z_YbTJx63Gj6uvnXJCAAJ9AAPFhdoNLmg3_4VAjKEeBA</t>
   </si>
   <si>
     <t xml:space="preserve">por que me persigue la desgracia | Por que nos persigue la desgracia </t>
   </si>
   <si>
-    <t>https://i.postimg.cc/XvhbQrW8/lossimpson-60635f75c23d0cd12017cb8129f30b1b-1200x800.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPymAJgvq3_tFCfEz88Z7Stq_vXiXQAAJ-AAPFhdoNf3PtAYKuPpMeBA</t>
   </si>
   <si>
-    <t>que mas ve?</t>
-  </si>
-  <si>
-    <t>https://postimg.cc/hf693Lpg</t>
+    <t>que mas ve? | que mas ve</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPzGAJgwOxi_O27CZ0gjAUpfdsyWuMAAJ_AAPFhdoN9qQLkJcV1S4eBA</t>
@@ -288,97 +190,64 @@
     <t>es un hechizo simple pero inquebrantable</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/13w5gcZQ/es-un-hechizo-simple-pero-inquebrantable2-2.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIPzmAJgw2sDch1x8xjE9Pv_l1a8h9KAAKAAAPFhdoNdy7e_-kRnfUeBA</t>
   </si>
   <si>
     <t>y volo</t>
   </si>
   <si>
-    <t>https://cdn.memegenerator.es/imagenes/memes/thumb/26/28/26280808.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP0GAJgxXh-m8ybuLMcrwElCOmZpHkAAKBAAPFhdoNyWBkc49M6gYeBA</t>
   </si>
   <si>
     <t>si bueno quien tiene hambre</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/505py01P/si-bueno-quien-tiene-hambre11564186254.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP0mAJgx6fXuTPi_JI4tCumFXQkvdDAAKCAAPFhdoNXZeTHF9mW8EeBA</t>
   </si>
   <si>
     <t>no lo se tu dime</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/1XwgsnQt/no-lo-se-tu-dime4.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP1GAJgyhLxOx916LSY-BniUj0DBj4AAKDAAPFhdoND9rJVyGNLM0eBA</t>
   </si>
   <si>
     <t>wey ya</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/cJwP7d03/wey-ya31580921271.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP1mAJgzO5IIBa6_QDQE1IDgABgIkbiwAChAADxYXaDU0y_plCEhXYHgQ</t>
   </si>
   <si>
     <t>ah caray eso si me interesa</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/j5Xd2Nj3/ah-caray-eso-si-me-interesa2.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP2GAJg0GjxmOhTM3-yuPU1RvvrA3PAAKFAAPFhdoNUu7xJ0GHofMeBA</t>
   </si>
   <si>
     <t>ya nos exhibiste</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/fRz4WFds/ya-nos-exhibiste2.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP2mAJg0m1u53r-uTW3Gg4ltAhXzcMAAKGAAPFhdoNxyAfdDnyzmQeBA</t>
   </si>
   <si>
     <t>lo logro</t>
   </si>
   <si>
-    <t>https://www.memegenerator.es/meme/31165286</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP3GAJg1PGsEbbYmJhC-DSeEw2vn2cAAKHAAPFhdoNNux324d3BfoeBA</t>
   </si>
   <si>
     <t>ve cerdo miserable</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/0yVKntZw/photo-2021-01-14-20-18-09.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP3mAJg1tAkNO2-xhhezOnsY-FsUUsAAKIAAPFhdoNl2XIa_dOkgseBA</t>
   </si>
   <si>
     <t>absolutely subarashi</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/BZwqmrGs/subarashi.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP4GAJg2U6zMSxKkvqKNxUxQWQWGA1AAKJAAPFhdoNHdV_Szyf8xAeBA</t>
   </si>
   <si>
-    <t>pasa algo?</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/25GnBkLn/STK-20190220-WA0017.png</t>
+    <t>pasa algo? | pasa algo</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIP4mAJg24kJIE6msK7TzfQ-RoAAXD5RQACigADxYXaDS4sA8SYOFOPHgQ</t>
@@ -387,16 +256,10 @@
     <t>ya me puse la pijama</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/dV42SRwz/STK-20190425-WA0024.png</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP5GAJg3ZhsU5N2iXpJJME7x7k-7FwAAKLAAPFhdoN21IycCeCvQoeBA</t>
   </si>
   <si>
-    <t>q se armen</t>
-  </si>
-  <si>
-    <t>https://postimg.cc/JtY6zd86</t>
+    <t>q se armen | que se armen</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIP5mAJg4HJPWdX9wAB3087HI8HLx6IpAACjAADxYXaDXv3m4GkcYWPHgQ</t>
@@ -405,81 +268,54 @@
     <t>no me digas que hacer</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/y6p4Bs9j/24883568-152148462076571-539314063090420184-o.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP6GAJg4q7rzXtOgs2MnbWNQO4hTXAAAKNAAPFhdoNT6jqwZbOcWMeBA</t>
   </si>
   <si>
     <t>te creo pero mi metralleta no</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/wj6GsrhM/69549469-409057799718968-5926320364647874560-o.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP6mAJg5KNkAtuwbtyyRa6_zXTCSGsAAKOAAPFhdoNPvllKSUlSvgeBA</t>
   </si>
   <si>
     <t>por que lo dice tan brusco</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/BnYMPnS7/Es-DSXNDVQAASFOH.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP7GAJg5rkMMbHFxePn1hsYdc8fYTtAAKPAAPFhdoN5B0TmaB0bDceBA</t>
   </si>
   <si>
     <t>que trucazo no</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/FHRxvXyy/Er-f-Y5v-WMAIju4.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP7mAJg6bRAV94W8vgGLwAAUAvFTvW4wACkAADxYXaDVgSGTLYexBaHgQ</t>
   </si>
   <si>
     <t>chucha ya</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/q7P3NbSL/url.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIP8GAJg61GasvgmSif0j2w2j3mEGlKAAKRAAPFhdoNDvNeBScVwNoeBA</t>
   </si>
   <si>
     <t>brutal</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/Y2N464Rf/brutal.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIQDmAJl1IOAl3oGtmXakGBzpaI4g4zAAKSAAPFhdoNiSoobGPtLuoeBA</t>
   </si>
   <si>
     <t>este men | ste men</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/TPmRHXJv/photo-2021-01-21-18-21-31.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIQp2AKFFT38CBb6yQxQRoSK2H-56XrAAKUAAPFhdoNh1fToIn_OFAeBA</t>
   </si>
   <si>
     <t>shut up and take my money | callate y toma mi dinero</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/ryYwmgmb/photo-2021-01-21-18-28-47.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIQqWAKFGZ6dWY_xe4wRpV_PFQ9oANSAAKVAAPFhdoNfnlSckGt_H4eBA</t>
   </si>
   <si>
     <t>esta informacion vale millones</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/pdZ2tJ4s/photo-2021-01-21-18-30-11.jpg</t>
-  </si>
-  <si>
     <t>CAACAgEAAxkBAAIQq2AKFHHKL3p3QDDpl_jjE30sHaaDAAKWAAPFhdoNdG60naG_GqIeBA</t>
   </si>
   <si>
@@ -492,7 +328,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>CAACAgEAAxkBAAISxmAMkgABs7D_UwnjBrxSrjI_OVftBwACEQEAAjyjtD8YqS8HDNCLRR4E</t>
+    <t>CAACAgEAAxkBAAIcOmAp85NNT8k1-n-e6T1QLwHzzQz9AAIRAQACPKO0PxipLwcM0ItFHgQ</t>
   </si>
   <si>
     <t>quede</t>
@@ -618,13 +454,13 @@
     <t>?</t>
   </si>
   <si>
-    <t>CAACAgEAAxkBAAIX5WAjIhQEBtUj5i66QdNOOHXtNgjcAAJmBQACrk3GKEUOqYYIQ4AgHgQ</t>
+    <t>CAACAgEAAxkBAAIcaGAp9GKcaMmGBskGTnodxT48uOeRAAJmBQACrk3GKEUOqYYIQ4AgHgQ</t>
   </si>
   <si>
     <t>el macho</t>
   </si>
   <si>
-    <t>CAACAgEAAxkBAAIX_GAjJFLw-V3508gxbWsbS43ZILfdAAIEAAPQ3xwZMulHv1ntYkgeB</t>
+    <t>CAACAgEAAxkBAAIcbGAp9WbTcFuJtdHbI_KHUn3LPfSkAAIEAAPQ3xwZMulHv1ntYkgeBA</t>
   </si>
   <si>
     <t>adios popo</t>
@@ -726,7 +562,7 @@
     <t>maldicion</t>
   </si>
   <si>
-    <t>CAACAgEAAxkBAAIY0mAkgpqQWUPr7APVjZEQQtrv3GvMAAKsAAPFhdoNEM-RgeYz1R4eBA</t>
+    <t>CAACAgEAAxkBAAIckWAp9lHxQVjDdMZoGDOH8t4i_lYoAAKiBQACrk3GKLrrZ38GKsm8HgQ</t>
   </si>
   <si>
     <t>mi corazon tiene pura maldad</t>
@@ -1000,30 +836,46 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIbaGApvqNlNuoh5LdqItpExJC-qBGXAALDAAMrc2AaMUv8jqoos94eBA</t>
+  </si>
+  <si>
+    <t>no mames que asco</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIc-2Ap-jCq3Jb08uwwy5XQ4AQ_SfgiAAJNAAOnMeM99tKj7rDXheYeBA</t>
+  </si>
+  <si>
+    <t>se va a estabilizar</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIg52Ay855dkUkNTvBysYBitMSah5gWAAIBAAPFhdoNaiEMiIMsREgeBA</t>
+  </si>
+  <si>
+    <t>que elegancia la de francia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIg72Ay9K3q_3Nsxggxl-vmuyULRTt0AAKxDAACRwABswLqKq6mPvmj7x4E</t>
+  </si>
+  <si>
+    <t>no creo | no no creo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIhEGAy-DC7604SOmORji0XyJz7rON-AAMBAAKnMeM9nEtWGx-X9hQeBA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1040,21 +892,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1085,40 +928,40 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1265,1338 +1108,2015 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="29.71"/>
+    <col customWidth="1" min="2" max="5" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="3" t="s">
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="s">
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="3" t="s">
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="3" t="s">
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="3" t="s">
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="s">
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B41" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="1" t="s">
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="3" t="s">
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="1" t="s">
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="3" t="s">
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="1" t="s">
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="3" t="s">
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B53" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="1" t="s">
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="3" t="s">
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="1" t="s">
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="3" t="s">
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="1" t="s">
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="3" t="s">
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B62" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="1" t="s">
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="3" t="s">
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B65" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="1" t="s">
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B46" s="3" t="s">
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B68" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="1" t="s">
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B48" s="3" t="s">
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B71" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="1" t="s">
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="3" t="s">
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="s">
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B74" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C51" s="1" t="s">
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="3" t="s">
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="A76" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="s">
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="s">
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="1" t="s">
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="A88" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="1" t="s">
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="1" t="s">
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="1" t="s">
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="1" t="s">
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="1" t="s">
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="1" t="s">
+    <row r="98" ht="15.75" customHeight="1">
+      <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="1" t="s">
+    <row r="99" ht="15.75" customHeight="1">
+      <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="1" t="s">
+    <row r="100" ht="15.75" customHeight="1">
+      <c r="A100" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="1" t="s">
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="A101" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="1" t="s">
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="A102" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="1" t="s">
+    <row r="103" ht="15.75" customHeight="1">
+      <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="1" t="s">
+    <row r="104" ht="15.75" customHeight="1">
+      <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="1" t="s">
+    <row r="105" ht="15.75" customHeight="1">
+      <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="1" t="s">
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="1" t="s">
+    <row r="107" ht="15.75" customHeight="1">
+      <c r="A107" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="1" t="s">
+    <row r="108" ht="15.75" customHeight="1">
+      <c r="A108" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="1" t="s">
+    <row r="109" ht="15.75" customHeight="1">
+      <c r="A109" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="1" t="s">
+    <row r="110" ht="15.75" customHeight="1">
+      <c r="A110" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="1" t="s">
+    <row r="111" ht="15.75" customHeight="1">
+      <c r="A111" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="s">
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
+    <row r="113" ht="15.75" customHeight="1">
+      <c r="A113" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="1" t="s">
+    <row r="114" ht="15.75" customHeight="1">
+      <c r="A114" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="s">
+    <row r="115" ht="15.75" customHeight="1">
+      <c r="A115" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="1" t="s">
+    <row r="116" ht="15.75" customHeight="1">
+      <c r="A116" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="1" t="s">
+    <row r="117" ht="15.75" customHeight="1">
+      <c r="A117" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="1" t="s">
+    <row r="118" ht="15.75" customHeight="1">
+      <c r="A118" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="s">
+    <row r="119" ht="15.75" customHeight="1">
+      <c r="A119" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="s">
+    <row r="120" ht="15.75" customHeight="1">
+      <c r="A120" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="s">
+    <row r="121" ht="15.75" customHeight="1">
+      <c r="A121" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="s">
+    <row r="122" ht="15.75" customHeight="1">
+      <c r="A122" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="s">
+    <row r="123" ht="15.75" customHeight="1">
+      <c r="A123" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="s">
+    <row r="124" ht="15.75" customHeight="1">
+      <c r="A124" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C100" s="1" t="s">
+    </row>
+    <row r="125" ht="15.75" customHeight="1">
+      <c r="A125" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="s">
+      <c r="B125" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C101" s="1" t="s">
+    </row>
+    <row r="126" ht="15.75" customHeight="1">
+      <c r="A126" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="1" t="s">
+    </row>
+    <row r="127" ht="15.75" customHeight="1">
+      <c r="A127" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C103" s="1" t="s">
+    </row>
+    <row r="128" ht="15.75" customHeight="1">
+      <c r="A128" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="s">
+      <c r="B128" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C104" s="1" t="s">
+    </row>
+    <row r="129" ht="15.75" customHeight="1">
+      <c r="A129" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="2" t="s">
+      <c r="B129" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C105" s="1" t="s">
+    </row>
+    <row r="130" ht="15.75" customHeight="1">
+      <c r="A130" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C106" s="1" t="s">
+    </row>
+    <row r="131" ht="15.75" customHeight="1">
+      <c r="A131" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C107" s="1" t="s">
+    </row>
+    <row r="132" ht="15.75" customHeight="1">
+      <c r="A132" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C108" s="1" t="s">
+    </row>
+    <row r="133" ht="15.75" customHeight="1">
+      <c r="A133" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="2" t="s">
+      <c r="B133" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C109" s="1" t="s">
+    </row>
+    <row r="134" ht="15.75" customHeight="1">
+      <c r="A134" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C110" s="1" t="s">
+    </row>
+    <row r="135" ht="15.75" customHeight="1">
+      <c r="A135" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="2" t="s">
+      <c r="B135" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C111" s="1" t="s">
+    </row>
+    <row r="136" ht="15.75" customHeight="1">
+      <c r="A136" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C112" s="1" t="s">
+    </row>
+    <row r="137" ht="15.75" customHeight="1">
+      <c r="A137" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C113" s="1" t="s">
+    </row>
+    <row r="138" ht="15.75" customHeight="1">
+      <c r="A138" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C114" s="1" t="s">
+    </row>
+    <row r="139" ht="15.75" customHeight="1">
+      <c r="A139" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C115" s="1" t="s">
+    </row>
+    <row r="140" ht="15.75" customHeight="1">
+      <c r="A140" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C116" s="1" t="s">
+    </row>
+    <row r="141" ht="15.75" customHeight="1">
+      <c r="A141" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C117" s="1" t="s">
+    </row>
+    <row r="142" ht="15.75" customHeight="1">
+      <c r="A142" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
+    </row>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="B11"/>
-    <hyperlink r:id="rId11" ref="B12"/>
-    <hyperlink r:id="rId12" ref="B13"/>
-    <hyperlink r:id="rId13" ref="B14"/>
-    <hyperlink r:id="rId14" ref="B15"/>
-    <hyperlink r:id="rId15" ref="B16"/>
-    <hyperlink r:id="rId16" ref="B17"/>
-    <hyperlink r:id="rId17" ref="B18"/>
-    <hyperlink r:id="rId18" ref="B19"/>
-    <hyperlink r:id="rId19" ref="B20"/>
-    <hyperlink r:id="rId20" ref="B21"/>
-    <hyperlink r:id="rId21" ref="B22"/>
-    <hyperlink r:id="rId22" ref="B23"/>
-    <hyperlink r:id="rId23" ref="B24"/>
-    <hyperlink r:id="rId24" ref="B25"/>
-    <hyperlink r:id="rId25" ref="B26"/>
-    <hyperlink r:id="rId26" ref="B27"/>
-    <hyperlink r:id="rId27" ref="B28"/>
-    <hyperlink r:id="rId28" ref="B29"/>
-    <hyperlink r:id="rId29" ref="B30"/>
-    <hyperlink r:id="rId30" ref="B31"/>
-    <hyperlink r:id="rId31" ref="B32"/>
-    <hyperlink r:id="rId32" ref="B33"/>
-    <hyperlink r:id="rId33" ref="B34"/>
-    <hyperlink r:id="rId34" ref="B35"/>
-    <hyperlink r:id="rId35" ref="B36"/>
-    <hyperlink r:id="rId36" ref="B37"/>
-    <hyperlink r:id="rId37" ref="B38"/>
-    <hyperlink r:id="rId38" ref="B39"/>
-    <hyperlink r:id="rId39" ref="B40"/>
-    <hyperlink r:id="rId40" ref="B41"/>
-    <hyperlink r:id="rId41" ref="B42"/>
-    <hyperlink r:id="rId42" ref="B43"/>
-    <hyperlink r:id="rId43" ref="B44"/>
-    <hyperlink r:id="rId44" ref="B45"/>
-    <hyperlink r:id="rId45" ref="B46"/>
-    <hyperlink r:id="rId46" ref="B47"/>
-    <hyperlink r:id="rId47" ref="B48"/>
-    <hyperlink r:id="rId48" ref="B49"/>
-    <hyperlink r:id="rId49" ref="B50"/>
-    <hyperlink r:id="rId50" ref="B51"/>
-    <hyperlink r:id="rId51" ref="B52"/>
-  </hyperlinks>
-  <drawing r:id="rId52"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed where blank spaces are stripped
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="281">
   <si>
     <t>Meme</t>
   </si>
@@ -55,7 +55,22 @@
     <t>CAACAgEAAxkBAAIbsmAp3jwXwIUGRxMw6uJDW6lvoNHzAAJnAAPFhdoNgFdzAypF_8oeBA</t>
   </si>
   <si>
-    <t>no puede ser</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">no puede ser | </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>hay | ay</t>
+    </r>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIbwGAp3yqz-_zYulzwwiPMDP_DLijrAAJpAAPFhdoNWMd92cV6AYgeBA</t>
@@ -65,12 +80,6 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPomAJgfNvkQwakOn_NA3gBsOdYfNHAAJqAAPFhdoNqadhusjy-toeBA</t>
-  </si>
-  <si>
-    <t>hay | ay</t>
-  </si>
-  <si>
-    <t>CAACAgEAAxkBAAIPpGAJggVYD5UWVNCQXz-Wu7jNFdNPAAJrAAPFhdoNAAG6b0TkGD33HgQ</t>
   </si>
   <si>
     <t>no</t>
@@ -1116,7 +1125,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="29.71"/>
-    <col customWidth="1" min="2" max="5" width="14.43"/>
+    <col customWidth="1" min="2" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1207,7 +1216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" ht="18.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1215,7 +1224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="18.75" customHeight="1">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2097,15 +2106,15 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>246</v>
@@ -2247,14 +2256,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
+    <row r="142" ht="15.75" customHeight="1"/>
     <row r="143" ht="15.75" customHeight="1"/>
     <row r="144" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Now linked stickers appear in inline query
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="291">
   <si>
     <t>Meme</t>
   </si>
@@ -163,7 +163,7 @@
     <t>CAACAgEAAxkBAAIPxmAJgtiMCJvplYnRXIROJ-81RCU8AAJ8AAPFhdoNYEjnFsDxL4EeBA</t>
   </si>
   <si>
-    <t xml:space="preserve">y ahora </t>
+    <t>esos no son</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIPyGAJgvKEP9Z_YbTJx63Gj6uvnXJCAAJ9AAPFhdoNLmg3_4VAjKEeBA</t>
@@ -866,13 +866,31 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIiK2A3J6S3y8kr-Q0Pl8-osvIQ355jAALMAAO96cFFPfEOV8rwoh0eBA</t>
+  </si>
+  <si>
+    <t>y ahora | y ahora? | ¿y ahora?</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIiQGA3MJ0T6oZfCnmpDt0Wo_BLNPzQAAIgAAPFhdoNozL7WHG6afYeBA | CAACAgEAAxkBAAIiQmA3MKbhpXKSWxPafBjIFNl6BQTEAAIhAAPFhdoNhf0gTTgqUUAeBA | CAACAgEAAxkBAAIiRGA3MKwks23eTHdHugbWPestq1zZAAIiAAPFhdoNJ7DkTKsET7geBA</t>
+  </si>
+  <si>
+    <t>me vale verga*</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIiTWA3MkPxDdyR6te5uTzsVg7aDpxPAALHAAPFhdoNMefIKi5yx-QeBA | CAACAgEAAxkBAAIiT2A3MkXoi3GN7KYKb0J5ZXDKigqpAALIAAPFhdoNp7j9ONRjbrgeBA | CAACAgEAAxkBAAIiUWA3MkhF1mHkiQWQaNe2syhd0TcXAALJAAPFhdoNzHqODZBNH1AeBA</t>
+  </si>
+  <si>
+    <t>i need you</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIiaGA3OfbjMHG_-IBUjOk7hS5Hi7ofAALUAAPFhdoNLdWWYKY6nYYeBA | CAACAgEAAxkBAAIiamA3OfhWMf_uMMADCu-AueU0i4J2AALTAAPFhdoNpbNkS3ptGZYeBA | CAACAgEAAxkBAAIibGA3Ofoh026trXupxeNEB-JXfdFWAALSAAPFhdoN9FkLZizXt8weBA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -881,6 +899,10 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -898,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -907,6 +929,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,7 +1354,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2272,9 +2297,30 @@
         <v>284</v>
       </c>
     </row>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1">
+      <c r="A144" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="145" ht="15.75" customHeight="1">
+      <c r="A145" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="146" ht="15.75" customHeight="1">
+      <c r="A146" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
     <row r="147" ht="15.75" customHeight="1"/>
     <row r="148" ht="15.75" customHeight="1"/>
     <row r="149" ht="15.75" customHeight="1"/>
@@ -3127,7 +3173,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Updated bersion for liberation
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="297">
   <si>
     <t>Meme</t>
   </si>
@@ -406,7 +406,7 @@
     <t>al fin un digno oponente</t>
   </si>
   <si>
-    <t>CAACAgEAAxkBAAIWhGAcVHK6lOuJveIQO9PF-bX31isbAAKdAAPFhdoNmGyQjL3bJRoeBA</t>
+    <t>CAACAgEAAxkBAAIWhGAcVHK6lOuJveIQO9PF-bX31isbAAKdAAPFhdoNmGyQjL3bJRoeBA | CAACAgEAAxkBAAIWhmAcVJHpZTL3eU_-TVofgEvepYWiAAKeAAPFhdoNffb48TGnDh8eBA</t>
   </si>
   <si>
     <t>nuestra batalla sera legendaria</t>
@@ -884,6 +884,24 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIiaGA3OfbjMHG_-IBUjOk7hS5Hi7ofAALUAAPFhdoNLdWWYKY6nYYeBA | CAACAgEAAxkBAAIiamA3OfhWMf_uMMADCu-AueU0i4J2AALTAAPFhdoNpbNkS3ptGZYeBA | CAACAgEAAxkBAAIibGA3Ofoh026trXupxeNEB-JXfdFWAALSAAPFhdoN9FkLZizXt8weBA</t>
+  </si>
+  <si>
+    <t>ya ya posi posi | ya posi</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIk5GA-6aPOAm9NGn_CdKdyUzg02j4jAAIaAAPFhdoNjc3L11hL4mAeBA</t>
+  </si>
+  <si>
+    <t>yo diria que si</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIk7GA-9wYGYm0sqcrK3O0QS7SurDZ2AALmAgACBTr4RcZstJDezOJ9HgQ</t>
+  </si>
+  <si>
+    <t>esa perra esta loca</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIk7mA-91HOSLrQZHOyJFtqCt8FnCedAAJeAQAClKP5RbHRpUZ8XrMVHgQ</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1695,7 @@
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2321,9 +2339,30 @@
         <v>290</v>
       </c>
     </row>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1">
+      <c r="A147" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="148" ht="15.75" customHeight="1">
+      <c r="A148" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="149" ht="15.75" customHeight="1">
+      <c r="A149" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
     <row r="150" ht="15.75" customHeight="1"/>
     <row r="151" ht="15.75" customHeight="1"/>
     <row r="152" ht="15.75" customHeight="1"/>
@@ -3172,7 +3211,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Added function to get webp file from photos
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="299">
   <si>
     <t>Meme</t>
   </si>
@@ -902,6 +902,12 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIk7mA-91HOSLrQZHOyJFtqCt8FnCedAAJeAQAClKP5RbHRpUZ8XrMVHgQ</t>
+  </si>
+  <si>
+    <t>soy el exito | y mirame soy el exito | mirame soy el exito</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAIm5mBFo8ajx2PQG3Ddn5MHC_IGbN8yAALiAAM2NihGeDb0buVV8h8eBA</t>
   </si>
 </sst>
 </file>
@@ -2363,7 +2369,14 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1">
+      <c r="A150" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
     <row r="151" ht="15.75" customHeight="1"/>
     <row r="152" ht="15.75" customHeight="1"/>
     <row r="153" ht="15.75" customHeight="1"/>
@@ -3210,7 +3223,6 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Update adding new memes
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="333">
   <si>
     <t>Meme</t>
   </si>
@@ -956,6 +956,60 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAIvCmBS2SHpZ8efFyq69Kkm7xNCCniFAAJQAQACfwyZRuZW85E_RJWlHgQ</t>
+  </si>
+  <si>
+    <t>la falta de respeto abunda por aquí | falta de respeto</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7EmB_Jg7ylTo7OuX768XDjWRZq8DaAAKEAQACFhT4R8OrJw7LLS6ZHwQ</t>
+  </si>
+  <si>
+    <t>fuera impulso de idiotez | impulso de idiotez | no fuera impulso de idiotez</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7FGB_JjH5EvUZGkrZBNG1NlDMjNE8AAISAQACHi75R5k_Ay8pdjtPHwQ</t>
+  </si>
+  <si>
+    <t>Cuantas veces tenemos que darle una leccion anciano | darle una leccion</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7FmB_Jl1X_ZyAfmTywPCy1Zs1jIhRAALUAQACsUD5R0xHerSaTa56HwQ</t>
+  </si>
+  <si>
+    <t>alan que pendejada hiciste | que hiciste</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7GGB_JoACCKnopQuVVd4xONC7ipWlAAKPAQAC4c34R05QjFIOVXvbHwQ</t>
+  </si>
+  <si>
+    <t>tuve ese sueño de nuevo | gary tuve ese sueño de nuevo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7GmB_JqAMdkcyGpILwieGLlimugIgAAKXAQACpAH5R8QXWC-dXoZgHwQ</t>
+  </si>
+  <si>
+    <t>mi lente de contacto | oh mi lente de contacto</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7HGB_JtlvA7p8p6A3B2CBKguDsPjUAALxAQACXEP5R7ZWljylnKu-HwQ</t>
+  </si>
+  <si>
+    <t>deja de hablar y pegale | pegale</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7HmB_JvEX1Fsld4tb8vDccdGJbbBhAAJXAQACWM0BRLaLkPndZ_QOHwQ</t>
+  </si>
+  <si>
+    <t>te parece que somos ricos</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7IGB_JwJ6AAFj7OQlovxDSAGc0iICEQACMgEAAqKb-EfauivMw5lHlR8E</t>
+  </si>
+  <si>
+    <t>demasiada comedia | no soportamos tanta comedia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAI7ImB_Jw_AjGb1Btul7XP2rgABCgVxWAACVQEAAvm6-EdKo9efOIHhJx8E</t>
   </si>
 </sst>
 </file>
@@ -2495,15 +2549,78 @@
         <v>314</v>
       </c>
     </row>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1">
+      <c r="A159" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="160" ht="15.75" customHeight="1">
+      <c r="A160" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="161" ht="15.75" customHeight="1">
+      <c r="A161" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="162" ht="15.75" customHeight="1">
+      <c r="A162" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="163" ht="15.75" customHeight="1">
+      <c r="A163" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="164" ht="15.75" customHeight="1">
+      <c r="A164" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="165" ht="15.75" customHeight="1">
+      <c r="A165" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="166" ht="15.75" customHeight="1">
+      <c r="A166" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="167" ht="15.75" customHeight="1">
+      <c r="A167" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
     <row r="168" ht="15.75" customHeight="1"/>
     <row r="169" ht="15.75" customHeight="1"/>
     <row r="170" ht="15.75" customHeight="1"/>
@@ -3329,7 +3446,6 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
New update and memes
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="465">
   <si>
     <t>Meme</t>
   </si>
@@ -211,7 +211,7 @@
     <t>CAACAgEAAxkBAAIP1mAJgzO5IIBa6_QDQE1IDgABgIkbiwAChAADxYXaDU0y_plCEhXYHgQ</t>
   </si>
   <si>
-    <t>ah caray eso si me interesa</t>
+    <t>ah caray eso si me interesa | eso si me interesa</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIP2GAJg0GjxmOhTM3-yuPU1RvvrA3PAAKFAAPFhdoNUu7xJ0GHofMeBA</t>
@@ -391,7 +391,7 @@
     <t>CAACAgEAAxkBAAIWbmAcJ0r--w39RKg8XUU40CqokT7vAAJjAAMjv0QoiTgh79EmxBUeBA</t>
   </si>
   <si>
-    <t>lo logre?</t>
+    <t>lo logre? | lo logre</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAIWcGAcJ3vq1cQw7ctGzizOyjPS2FvVAAKIAAMjv0QoS4oY4OZCitweBA</t>
@@ -1216,7 +1216,7 @@
     <t>CAACAgEAAxkBAAJwWmEIhBNZVVhTJqV6Tifx7IF2dk2HAAJHAQACZy9ARLNKd8Md-OzpIAQ</t>
   </si>
   <si>
-    <t>espera lo dices en serio? | ah espera lo dices en serio? | dejame reir mas fuerte</t>
+    <t>espera lo dices en serio? | ah espera lo dices en serio? | dejame reir mas fuerte | espera lo dices en serio | ah espera lo dices en serio</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAJ0OGFno3sS0yTTzd8x6Em-04EhmkPMAALhAQACc4tARwgCbltta8BuIQQ | CAACAgEAAxkBAAJ0OmFno_va97l8Bh_zB4NuOLZdxcu0AAKyAQACOKo4R4gso37McVbTIQQ</t>
@@ -1286,6 +1286,126 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAJ2Q2Fs7AABa5ZOuHnVFkN3LzCzKnA7pQAC-gEAAqiBaEft2nrPE7Rn0CEE</t>
+  </si>
+  <si>
+    <t>inteligente no | inteligente no?</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAJ3l2FwmVIs2lx5Wr6MAaEx1QgOLYkmAAJuAQACU_mIR9bLPtWLt6QcIQQ</t>
+  </si>
+  <si>
+    <t>vaya no encuentro fallas en su logica | no encuentro fallas en su logica</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAJ_cmGee9KcWEZ7RsVrL3OpU0ByZAdpAAISAgACEuHxRFIZkK12wOenIgQ</t>
+  </si>
+  <si>
+    <t>crei que teniamos algo | crei que teniamos algo especial</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAJ_dGGee9ujocFa3AVcOQELDuzqLdBwAAJHAwACJCP5RFpUofZqp1mTIgQ</t>
+  </si>
+  <si>
+    <t>echele ganas mijo | metele ganas</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKACmGiz6OOasz9ikl6jBDOGyblmyqvAAJWAgACh54ZRd35i0_x_6XBIgQ</t>
+  </si>
+  <si>
+    <t>señor calamardo venga a ver esto</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKALmGi1hrAkbt1dgABQuhkbo03YwSKigACPgADxYXaDTaeEOp5ifDdIgQ | CAACAgEAAxkBAAKAMGGi1iK9LXZQc_KE_cf1LJwRzMWDAAI_AAPFhdoN7A9UBDj08TgiBA</t>
+  </si>
+  <si>
+    <t>con resultados sexuales | terminara con resultados sexuales</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKAN2Gi2K-9L533-Id4joo4eiKowtZaAAL4AQACVSUZRS6grsvfVaveIgQ</t>
+  </si>
+  <si>
+    <t>no somos cavernicolas tenemos tecnologia | no somos cavernicolas | tenemos tecnologia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKBZ2GxWxJBQoCq-ffez5iIsJi58dWbAALoAQACqpWIRTxGaMBo1B1bIwQ | CAACAgEAAxkBAAKBaWGxW3k8L0dU6HsaT7UEDEYafAxJAAKkAgACAu2IRdt8kYn11lAEIwQ | CAACAgEAAxkBAAKBa2GxW4Nw7xAFbMkAAVA6XkeC-8020wACsgIAAlHxiEVUzCyYNPwnliME | CAACAgEAAxkBAAKBbWGxW9AzL4EiWDnf5c8FDu8dY2cJAALWAgACgpaIRS-MO889ut1BIwQ</t>
+  </si>
+  <si>
+    <t>viva cristo rey | cristo rey</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKBb2GxW9tA7a9CREEWuzkY8YkyGYZZAAL9AQAC0sOJRTPThjiwGCMGIwQ</t>
+  </si>
+  <si>
+    <t>ya es algo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKBcWGxW--ihCDu7ItSTcusQ67kq4gyAAKUAQAC4DSRRdBdDpKzUKaUIwQ</t>
+  </si>
+  <si>
+    <t>por un demonio lo que faltaba | por un demonio</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE3GHXckaDCKVKFVtD8kfsCTaS4ItKAAI7AQAC6Q-4RmVQO2Lwoz5YIwQ</t>
+  </si>
+  <si>
+    <t>pana | panas</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE3mHXcmPSSfFczglCRfHFkuYcXKiwAALIAQAC7hq4RjPiZw_zUHI2IwQ</t>
+  </si>
+  <si>
+    <t>soy una verguenza | soy una verguenza para mi especie | soy una vergüenza | soy una vergüenza para mi especie</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE4GHXcnSALmUsPC5H9h-78B84wVb1AAKvAQAC3zfARuDX5ulbAnMCIwQ</t>
+  </si>
+  <si>
+    <t>premio nobel | premio nobel otto premio nobel</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE4mHXcsjA9tqGmRbzYfUIpck70lpdAAIWAgACxPi4Rr39DdqGEa6-IwQ</t>
+  </si>
+  <si>
+    <t>vaya ese tipo si que esta loco | ese tipo esta loco | estas loco</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE5GHXct8TZophVPfmycihmEyjWWHvAAL8AQACyc-5RvlhU9-wb9EYIwQ</t>
+  </si>
+  <si>
+    <t>oye si vas a empezar con tus homosexualidades no puedes jugar | si vas a empezar con tus homosexualidades no puedes jugar</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE5mHXcwPK9o06F5z4UPdxqY4wEKezAAKIAgACyEfBRtgosvR4P8T2IwQ</t>
+  </si>
+  <si>
+    <t>que pro | q pro</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE6GHXcyVOh1HTBu3oBs6HQ5S9Pg4VAAJRAgAC9ijARpuTmXFcFJYoIwQ</t>
+  </si>
+  <si>
+    <t>asi lo quizo la tva | asi lo quizo la tva mijo | asi lo quizo la tva mijo no este chingando</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE6mHXczI3iCTomzbIXXNcsGr-LuRHAALRAQACrYfBRgRQgThQY7OPIwQ</t>
+  </si>
+  <si>
+    <t>conchetumadre | ctm</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE7GHXc2Y5xGVLRejihqM8F71JpgLCAAKMAQAC73_ARtnynpQhBS0ZIwQ</t>
+  </si>
+  <si>
+    <t>oye tranquilo viejo | tranquilo viejo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE8GHXdEy6tOnI2baHD87MdsYMNEKNAAJ3AgACIl24RlfBxlo2um8MIwQ</t>
+  </si>
+  <si>
+    <t>estas retandome | estas retandome? | que? estas retandome? | que estas retandome?</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKE-2HXtkcQMhLKHnpkYu9so-uQgZm5AAJaAgACplnBRqrYH_tW2G3RIwQ</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +1963,7 @@
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2083,7 +2203,7 @@
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -3282,26 +3402,166 @@
         <v>424</v>
       </c>
     </row>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1">
+      <c r="A214" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="215" ht="15.75" customHeight="1">
+      <c r="A215" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="216" ht="15.75" customHeight="1">
+      <c r="A216" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="217" ht="15.75" customHeight="1">
+      <c r="A217" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="218" ht="15.75" customHeight="1">
+      <c r="A218" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="219" ht="15.75" customHeight="1">
+      <c r="A219" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="220" ht="15.75" customHeight="1">
+      <c r="A220" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="221" ht="15.75" customHeight="1">
+      <c r="A221" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="222" ht="15.75" customHeight="1">
+      <c r="A222" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="223" ht="15.75" customHeight="1">
+      <c r="A223" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="224" ht="15.75" customHeight="1">
+      <c r="A224" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="225" ht="15.75" customHeight="1">
+      <c r="A225" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="226" ht="15.75" customHeight="1">
+      <c r="A226" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="227" ht="15.75" customHeight="1">
+      <c r="A227" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="228" ht="15.75" customHeight="1">
+      <c r="A228" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="229" ht="15.75" customHeight="1">
+      <c r="A229" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="230" ht="15.75" customHeight="1">
+      <c r="A230" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="231" ht="15.75" customHeight="1">
+      <c r="A231" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="232" ht="15.75" customHeight="1">
+      <c r="A232" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="233" ht="15.75" customHeight="1">
+      <c r="A233" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>464</v>
+      </c>
+    </row>
     <row r="234" ht="15.75" customHeight="1"/>
     <row r="235" ht="15.75" customHeight="1"/>
     <row r="236" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added ban/unbann options (not tested yet)
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="467">
   <si>
     <t>Meme</t>
   </si>
@@ -1406,6 +1406,12 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAKE-2HXtkcQMhLKHnpkYu9so-uQgZm5AAJaAgACplnBRqrYH_tW2G3RIwQ</t>
+  </si>
+  <si>
+    <t>taweno</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKFImHhu5DzB3td6bNL95Eh6SWXCKUAAzcAA8WF2g2-rpNPmi-B0CME</t>
   </si>
 </sst>
 </file>
@@ -3562,7 +3568,14 @@
         <v>464</v>
       </c>
     </row>
-    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1">
+      <c r="A234" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>466</v>
+      </c>
+    </row>
     <row r="235" ht="15.75" customHeight="1"/>
     <row r="236" ht="15.75" customHeight="1"/>
     <row r="237" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added converter to generate video stickers
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="529">
   <si>
     <t>Meme</t>
   </si>
@@ -1408,10 +1408,196 @@
     <t>CAACAgEAAxkBAAKE-2HXtkcQMhLKHnpkYu9so-uQgZm5AAJaAgACplnBRqrYH_tW2G3RIwQ</t>
   </si>
   <si>
-    <t>taweno</t>
+    <t>taweno | ta bueno</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAKFImHhu5DzB3td6bNL95Eh6SWXCKUAAzcAA8WF2g2-rpNPmi-B0CME</t>
+  </si>
+  <si>
+    <t>fino señores | fino</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYnmJ6iEQx16bDPiv_Zk-T8eErj5PfAAI2AwACz5TRRwQWtGItC9rzJAQ</t>
+  </si>
+  <si>
+    <t>un clasico | clasico</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYoGJ6iFKC6gM1A24egnKmtTGGjbWSAAKGAgACXOnZR9ugI6YifSYPJAQ</t>
+  </si>
+  <si>
+    <t>Por que no me muero</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYomJ6iHLn8KVYVkD0PA2AC2ODAAGilQACrwEAAmzl0EfznyZBVvMFayQE</t>
+  </si>
+  <si>
+    <t>siempre espera lo inesperado | espera lo inesperado</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYpGJ6iIkE9L8eovhds9nrpwWsx4ylAALHAQACD9_YR3fm0WEq6sAVJAQ</t>
+  </si>
+  <si>
+    <t>algo anda mal</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYqGJ6iPlPiufwmlO3zsr7eLwKyQqvAAKOAgAC0LjQRwU7oeZ8Xt4nJAQ</t>
+  </si>
+  <si>
+    <t>estuviste practicando | estuviste practicando eh</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYqmJ6iQXX05Kno-OX60bgrUn6ftjKAAJUAwAC88TRR967aBO56HNIJAQ</t>
+  </si>
+  <si>
+    <t>ya no quiero verte nunca mas</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYrGJ6iRhnrFVQ3s0Glku_uqGPRgSGAAIZAgAC5I_RR0d9A0gIo4PNJAQ</t>
+  </si>
+  <si>
+    <t>bien pensado woody | bien pensado</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYrmJ6iSiD-Ph0eXxQhrYP-ZW4EhKNAAJCAgACDiTZR0aQ52guLvymJAQ</t>
+  </si>
+  <si>
+    <t>debe haber un mensaje oculto en algun lado</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYsGJ6iTtPhFZ8kPB8CF39hJLBjhB4AAL3BQACNKLQR7QiSv-s8bKgJAQ</t>
+  </si>
+  <si>
+    <t>adinivare escuela publica | escuela publica?</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYsmJ6iVA2ZrRZS0YC1g7K7ZdD-yicAAJqAgACYiHRRybYHd7jZ7XiJAQ</t>
+  </si>
+  <si>
+    <t>que pendejo | pendejo | bien pendejo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYtGJ6iWf2dgWtNFaeGhLD5yiwiuwDAAIHAgACqgXYR_F5M_vV5nRFJAQ</t>
+  </si>
+  <si>
+    <t>yo no recibo ordenes | yo no recibo ordenes de ti | soy un prime yo no recibo ordenes de ti</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYtmJ6iYB_6WUTDu8EGLRsc3dXqYA5AAIFAwAC-jXYRzbXRJG6bBIwJAQ</t>
+  </si>
+  <si>
+    <t>chingues a tu madre</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYuGJ6iaf1-S-q5R696tl3pepMYXznAAKxAgACSE3ZR1Jp-2qiDk2QJAQ</t>
+  </si>
+  <si>
+    <t>las cosas se salieron de control</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYumJ6ibVWLKDWhicUbr0LSRgvOSVkAAJ3AgAC0CDZR3KDm6bifm8lJAQ</t>
+  </si>
+  <si>
+    <t>norman se fue de sabatico | se fue se sabatico | norman se fue de sabatico cariño</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYvGJ6icMFICUY1uR0I_hVAkrnTMM3AAKFAgACwfXRRywaOzhLEx9xJAQ</t>
+  </si>
+  <si>
+    <t>apagalo otto | apagalo otto apagalo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYvmJ6idoPsC3Tr5MJnqGJj5cDTskbAALVAQAC9GzRR7ZV9S4QakdLJAQ</t>
+  </si>
+  <si>
+    <t>te convertiste en aquello que juraste destruir</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYwGJ6ieqYwhLW9l8QqNSF0OsVriteAALYAQACXGHYRxvjCFmihjrXJAQ</t>
+  </si>
+  <si>
+    <t>acompañame a ver esta triste historia | esta triste historia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYwmJ6iiH05krRZekYLrLCsaqzyH3qAAIPAgAC9tfZR1jHe_5ngytbJAQ</t>
+  </si>
+  <si>
+    <t>ya no hijo no te creo | no te creo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYxGJ6ikvscJegPShuDH5mSFaYQcnxAAIbAgACUeXQR499OJhOSkwAASQE</t>
+  </si>
+  <si>
+    <t>primera vez</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYymJ6i9wAAbYjMRv--cB8wI9Z4iT_HAACHAIAAjr32EdYdqbqqhF0RSQE</t>
+  </si>
+  <si>
+    <t>cuanta virgindad hay en este mundo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKYzGJ6i-vNBvCeeQ3oCGgTbWJRYkYHAAJjAwACkhzRR2z7JrhL1e33JAQ</t>
+  </si>
+  <si>
+    <t>nel</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKaumKDSUnRGEQjfMQdX682-ByY63sOAAJxAgAC284YRKLIe-5NKoKYJAQ</t>
+  </si>
+  <si>
+    <t>yo te conozco</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKavGKDSXmOurwJrmwaiGhtOzZbm-0sAAJAAwACczoYROdUjUNYoprbJAQ</t>
+  </si>
+  <si>
+    <t>que se armen los pinches chingadazos | que se armen</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKavmKDSYavYJfvqAIqDs-l1FcRoGxOAAJMAgAC5zcZRPOHQ_snEfetJAQ</t>
+  </si>
+  <si>
+    <t>corre perra corre</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKawGKDSaa8u8rh8QeCgweeW8SxawQkAAIfAgAC6cMYRFCinDUjQcOWJAQ</t>
+  </si>
+  <si>
+    <t>lo voy a gozar</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKawmKDSbgcqCoo5iMYYuaViyh4DgU0AALFAgACrgUZRM1F_oBmJYN1JAQ</t>
+  </si>
+  <si>
+    <t>besitos besitos chau chau</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKaxGKDScWmNTZ5OJKhF7inUqLKqPW5AALjAgACfG4YRDBqUQrUUmSWJAQ</t>
+  </si>
+  <si>
+    <t>le falle señor | le falle | le falle señor ud confió en mi y yo le falle | ud confio en mi y yo le falle</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKaxmKDSdQguJfFnnK9Yz8-VqWkxzKRAAINAwAC37wYRDwz3FbdcjwSJAQ</t>
+  </si>
+  <si>
+    <t>valio madres | ya valio madres</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKayGKDSfljGeVupdp6TF1L4Rkudco_AAKDAwACqyEZRLgBZeV5MIg2JAQ</t>
+  </si>
+  <si>
+    <t>obvio</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKaymKDSgkznlteVbYTrY6BghO5eO4fAAK3AQAC6iwhRB0MhmFrlUETJAQ</t>
+  </si>
+  <si>
+    <t>unlimited power</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKazGKDShMnDI8rm45-pE_AHu1jiFz4AALNAgACOKEZRJyc5mNdrGO-JAQ</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1608,8 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1446,6 +1633,7 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3576,37 +3764,254 @@
         <v>466</v>
       </c>
     </row>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1">
+      <c r="A235" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="236" ht="15.75" customHeight="1">
+      <c r="A236" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="237" ht="15.75" customHeight="1">
+      <c r="A237" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B237" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="238" ht="15.75" customHeight="1">
+      <c r="A238" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="239" ht="15.75" customHeight="1">
+      <c r="A239" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="240" ht="15.75" customHeight="1">
+      <c r="A240" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="B240" s="6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="241" ht="15.75" customHeight="1">
+      <c r="A241" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B241" s="6" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="242" ht="15.75" customHeight="1">
+      <c r="A242" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="243" ht="15.75" customHeight="1">
+      <c r="A243" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B243" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="244" ht="15.75" customHeight="1">
+      <c r="A244" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B244" s="6" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="245" ht="15.75" customHeight="1">
+      <c r="A245" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="B245" s="6" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="246" ht="15.75" customHeight="1">
+      <c r="A246" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="247" ht="15.75" customHeight="1">
+      <c r="A247" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="248" ht="15.75" customHeight="1">
+      <c r="A248" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="249" ht="15.75" customHeight="1">
+      <c r="A249" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="250" ht="15.75" customHeight="1">
+      <c r="A250" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="251" ht="15.75" customHeight="1">
+      <c r="A251" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="252" ht="15.75" customHeight="1">
+      <c r="A252" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="253" ht="15.75" customHeight="1">
+      <c r="A253" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B253" s="6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="254" ht="15.75" customHeight="1">
+      <c r="A254" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="255" ht="15.75" customHeight="1">
+      <c r="A255" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="256" ht="15.75" customHeight="1">
+      <c r="A256" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="B256" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="257" ht="15.75" customHeight="1">
+      <c r="A257" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="B257" s="6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="258" ht="15.75" customHeight="1">
+      <c r="A258" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="B258" s="6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="259" ht="15.75" customHeight="1">
+      <c r="A259" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B259" s="6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="260" ht="15.75" customHeight="1">
+      <c r="A260" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="261" ht="15.75" customHeight="1">
+      <c r="A261" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="262" ht="15.75" customHeight="1">
+      <c r="A262" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B262" s="6" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="263" ht="15.75" customHeight="1">
+      <c r="A263" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="264" ht="15.75" customHeight="1">
+      <c r="A264" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B264" s="6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="265" ht="15.75" customHeight="1">
+      <c r="A265" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="B265" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
     <row r="266" ht="15.75" customHeight="1"/>
     <row r="267" ht="15.75" customHeight="1"/>
     <row r="268" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Refactored followed sonarlint suggestions
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="629">
   <si>
     <t>Meme</t>
   </si>
@@ -1534,7 +1534,7 @@
     <t>CAACAgEAAxkBAAKYymJ6i9wAAbYjMRv--cB8wI9Z4iT_HAACHAIAAjr32EdYdqbqqhF0RSQE</t>
   </si>
   <si>
-    <t>cuanta virgindad hay en este mundo</t>
+    <t>cuanta virginidad hay en este mundo</t>
   </si>
   <si>
     <t>CAACAgEAAxkBAAKYzGJ6i-vNBvCeeQ3oCGgTbWJRYkYHAAJjAwACkhzRR2z7JrhL1e33JAQ</t>
@@ -1598,6 +1598,306 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAKazGKDShMnDI8rm45-pE_AHu1jiFz4AALNAgACOKEZRJyc5mNdrGO-JAQ</t>
+  </si>
+  <si>
+    <t>uhy asi que chiste | asi que chiste</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKa_2KEWmbCnrxemeVSZo0XpZJhp2UmAAJMAgACHzMZRH3TliKHY_x2JAQ</t>
+  </si>
+  <si>
+    <t>esta bien a ver si contesta alguien que no sea un retrasado | a ver si contesta alguien que no sea un retrasado</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbAWKEWo6tZDaQ8uCWfRc-eyHX1thPAAKhAgACmbkZRNwQlawFb1JLJAQ</t>
+  </si>
+  <si>
+    <t>sr stark ahora que hago | ahora que hago? | ahora que hago</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbA2KEWrWbtnf3epnYL5mnV48nBjgvAALwAgAC0J4ZRLmF-KaNcY_BJAQ</t>
+  </si>
+  <si>
+    <t>mi mente es superior a la de los demas | mi mente es superior | mente superior</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbBWKEWto1JVQPuHH2FBzHgH4drki6AAJrAgAC_F4hRBnr9sFpJUKuJAQ</t>
+  </si>
+  <si>
+    <t>fuersa bro | fuerza bro</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbNmKEYO8fIqjtZ61JZhNVo0Q9W8TrAALIAQACT98hRCFLCY1RYdrCJAQ</t>
+  </si>
+  <si>
+    <t>por que no se mueren | puedo destruir galaxias con un pensamiento por que no se mueren</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbOGKEYP_fDpwYruE-MuDx_914F0HgAAKaAgACcpkhRAABOon-qPDlHyQE</t>
+  </si>
+  <si>
+    <t>pero las risas no faltaron | pero las risas no faltaron eh</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbOmKEYVfyMFs_tU7qHrXkkHIWrK45AAI_AgACbQMhRCoOAWHJlMUnJAQ</t>
+  </si>
+  <si>
+    <t>no puede ser</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbPGKEYXTndXk558vBOC86YAVW7KNRAAL_AgACpV4gRN7E2b2X_brmJAQ</t>
+  </si>
+  <si>
+    <t>mis mejores amigos</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbPmKEYYEAAXe9QGKgZ7lrDTeJmt46dwAC1QIAAlB3IUS08rtouuXmXiQE</t>
+  </si>
+  <si>
+    <t>va a suceder otra vez</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbQGKEYY7dqYeJR7HSrgpBFzrp3FirAALjAQACDrQoRLFOPJhIR7yCJAQ</t>
+  </si>
+  <si>
+    <t>esto ya es otro nivel | esto ya es la hostia | esto ya es otro nivel esto es la hostia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbQmKEYZ3xYDQ6sflPnj40783O_wcEAAJ1AgACxakgRPjKSNcNd9KFJAQ</t>
+  </si>
+  <si>
+    <t>con que derecho lo dices tu</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbRGKEYcMx9iMngTN_A5VrZaZdHRw8AALOAgACuHUgRI9aNZbdC0gPJAQ</t>
+  </si>
+  <si>
+    <t>este es el fin de sid | este es el fin | este es el fin de sid el perezoso</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbRmKEYdFON7UJBV8KBs53D7I7tOvBAAIrAgACR_AgRPy2xGJS2dAcJAQ</t>
+  </si>
+  <si>
+    <t>magnifico | magnifico magnifico magnifico</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbSGKEYe0jKwGv4qRNl8898ZRJNEmvAAIdAgACuSEgRIh9YKmnHmFpJAQ</t>
+  </si>
+  <si>
+    <t>que macizo | cielos que macizo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbSmKEYgYVQS2X_KaM04hBPfGcvDiiAAKjAgACAdQpRGep43nfCFiiJAQ</t>
+  </si>
+  <si>
+    <t>esa no me la esperaba | eso no me lo esperaba</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbTGKEYhtplc8qnVdkczkzBQ3RpoX2AAIvAgACZhUhRDmBEGAY3ha3JAQ</t>
+  </si>
+  <si>
+    <t>eso si es de gansters | joder eso si es de gangsters</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbTmKEYi7tDSB7AUm8-Qijiw9a4nx2AAK1AgACO04pRKLY1jGQmbHqJAQ</t>
+  </si>
+  <si>
+    <t>estoy agarrando señal | estoy agarrando senal</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbUGKEYkujLIIOkpOwCb4VcV8VD_9pAAKcAQACyYYpRDrLX0eU8VjLJAQ</t>
+  </si>
+  <si>
+    <t>lo guardo solo para emergencias | solo para emergencias</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbUmKEYnDnSJexa1yCvLhrnK-9AnWlAAJkAgACFX4hRFFJ3ct2rtMDJAQ</t>
+  </si>
+  <si>
+    <t>tienes tantos estilos</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbVGKEYoSOjASdc9q-smOKnjr0-gEmAAJiAwACU5YpRJjO8ESox2FAJAQ</t>
+  </si>
+  <si>
+    <t>que gran historia | joder que gran historia</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbVmKEYpEHZLZVJZ8HNE-ikRLs28YqAAIaAgAChZopRLcaKMmMLhGLJAQ</t>
+  </si>
+  <si>
+    <t>si esta potente el olorcito | potente el olorcito</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbWGKEYqPHifuVNpAydQaw9jGcOZ-tAAKBAwACv8AgRF6f-CxHGtflJAQ</t>
+  </si>
+  <si>
+    <t>haz comenzado una guerra que es imposible que ganes | es imposible que ganes</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbWmKEYriRluBReZl48PZK98BBcwf6AAJ6AQACQn4oRDYSmu4cEwYKJAQ</t>
+  </si>
+  <si>
+    <t>pa que te digo no si si | pues pa que te digo no si si | para que te digo no si si | pues para que te digo no si si</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbXGKEYxTYDP9cMlVyAAH3oOniYM6opAACaQIAAvboKURLgAevT52WCyQE</t>
+  </si>
+  <si>
+    <t>te lo agradezco peter | te lo agradezco peter eres la unica familia que tengo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbYmKEZRTKXeLomPR_AAHTEc0L17HHwQACngEAAps_KUQw2SRQqEjfDCQE</t>
+  </si>
+  <si>
+    <t>peter parker</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKbZmKEZZB9we6e3nDtEnJyhgSIn_NEAALOAgACPB4hRBJwRdWpknGVJAQ</t>
+  </si>
+  <si>
+    <t>te lo juro por dieguito maradona | te lo juro por maradona | te lo juro por diego maradona</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsEGLQ0cYrAVRhYbwyLEsu8RQsVw36AAJ5AgAClf4BRpX8eRUFh9KWKQQ</t>
+  </si>
+  <si>
+    <t>estoy en esta foto y no me gusta | im in this photo and i dont like it | im in this photo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsEmLQ0gZaDniO6cGICD16i4H1FJqpAAJiAgACep8AAUbPNJ1yTgABRvkpBA</t>
+  </si>
+  <si>
+    <t>no digas mamadas | no digas mamadas mary jane | no digas mamadas maijain</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsFGLQ0jCIHU-faiH99x5k5rnwSc6_AAImAwACqg0BRqd4TyWewf8NKQQ</t>
+  </si>
+  <si>
+    <t>super f</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsFmLQ0myF37oqrQqixodUeUlbc195AAMDAALrQgABRlTB2-4S9aC5KQQ</t>
+  </si>
+  <si>
+    <t>te crees muy gracioso | imbecil te crees muy gracioso</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsGGLQ0nraRSe0lwzpVwSrywiyaGoAA4cCAAILdwFGepEKrahKhNIpBA</t>
+  </si>
+  <si>
+    <t>espera eso es ilegal | wait thats illegal</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsGmLQ0pkQmtcUEYAb2ixp-MDrza-YAAJOAgACF9QAAUbyThuPFUMjvikE</t>
+  </si>
+  <si>
+    <t>no me pidas que deje de ser hombre</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsHGLQ0rNZQFyCr96Ns7OCLQSADZbEAAKBAgACvSMBRutVp6bXsgABVykE</t>
+  </si>
+  <si>
+    <t>pero que imbecil | que imbecil</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsKGLQ1AQM3w2uL4TCvBkehHmMqFR4AAIvAgACb3kAAUY8uTtQLJVMSykE</t>
+  </si>
+  <si>
+    <t>pense que el chat era de hombres lobo no de niños rata</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsPmLQ2QyRpLi2ObVIBqerGpQTwZqgAAIFAwACBKyrB9A84oE0TAHyKQQ</t>
+  </si>
+  <si>
+    <t>no me des esperanza | no no me des esperanza</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsUGLQ20gR35l_lhjbSHvKEQcYhnOCAAJBAgACJcyJRsELmA4rCXqeKQQ</t>
+  </si>
+  <si>
+    <t>de poeta a poeta | dejeme estrechar su mano | dejeme estrechar su mano de poeta a poeta</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsUmLQ212r6vj5fsgsG8M4lW4Gp7WWAAKIAgACxN-IRqF22PwO7vFtKQQ</t>
+  </si>
+  <si>
+    <t>por que no puedo ser tu</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsVGLQ23sMeSCq0Gexlye5hufkHEw1AAL3AQAChoGARqeGIMulj68dKQQ</t>
+  </si>
+  <si>
+    <t>silencio cara de la buena | silencio crvrg | silencio crv</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsVmLQ24xfe65pQnONh_cI68Zd6ieYAALTAwACzM6IRmPjw9bFMBujKQQ</t>
+  </si>
+  <si>
+    <t>lo apoyo</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsWGLQ26vrDD-8PuSCL8gHYJrhb9MkAAKVAgAC9AqIRm677iTusEhUKQQ</t>
+  </si>
+  <si>
+    <t>el tiempo se acaba | el tiempo se acaba esponja</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsWmLQ271PxZZVR4gDiLl7XCk-JsI8AAKcAgACeGKIRnvVl7NT27EZKQQ</t>
+  </si>
+  <si>
+    <t>mi manera es la manera de los dioses | mi manera es la de los dioses</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsXGLQ29AZxJh0nAKNE0NRYie7PxG1AAJlAwACTyuJRveuG24VVSwMKQQ</t>
+  </si>
+  <si>
+    <t>que belleza mi pana | belleza | que belleza</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsXmLQ2-zUfDeREUOVHEJFfI9FWvoOAAJUAgAC6NmJRrW_D3ZV1GNXKQQ</t>
+  </si>
+  <si>
+    <t>aqui no hacemos eso | aqui no hacemos esas cosas</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsYGLQ3AX9b7xSVzJKb-S-blzUXotgAAIWAgACCWKJRlYOwL34Tx3CKQQ</t>
+  </si>
+  <si>
+    <t>fucking hippie motherfuckers | pinches hippies | malditos hippies</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsYmLQ3BkfGpOl2qe-9sFdeE_SzsJEAAIJAgACeXGIRmCZ9tgviS1nKQQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ud callese | usted callese | ud callese que es bailarina | ud es bailarina | usted es bailarina | usted callese que es bailarina | usted callese que usted es bailarina </t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsZGLQ3DnF_MW-kamTn6KW7h6d-aR3AAKQAgACyb2JRk2d5RYwccyGKQQ</t>
+  </si>
+  <si>
+    <t>zapatero a sus zapatos</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsZmLQ3H5v8WSknPVzxNBpJCUvbO3-AAITAwAClDWJRn9sqSCv3dgiKQQ</t>
+  </si>
+  <si>
+    <t>delete this | sonrie y borra esto</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsaGLQ3I42S1bR5s_gMBxsSAPDDv1QAAL3AgACoESBRiYNXp2sVP4NKQQ</t>
+  </si>
+  <si>
+    <t>el poder del sol en la palma de mi mano | el poder del sol | en la palma de mi mano</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsamLQ3KQdb8YyGiS4BdSnimB_5YIRAALSAgACfjGIRoXSfkPpZZ6xKQQ</t>
+  </si>
+  <si>
+    <t>esta parte de mi vida se llama felicidad | esta parte esta pequeña parte se llama felicidad | se llama felicidad | esto se llema felicidad | esto es felicidad</t>
+  </si>
+  <si>
+    <t>CAACAgEAAxkBAAKsbGLQ3L2oCJo8QxbinGQEh8Bv9J6aAAL1AQACHCeJRnu9iot1Ezk3KQQ</t>
   </si>
 </sst>
 </file>
@@ -4012,56 +4312,406 @@
         <v>528</v>
       </c>
     </row>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1">
+      <c r="A266" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="267" ht="15.75" customHeight="1">
+      <c r="A267" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="B267" s="6" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="268" ht="15.75" customHeight="1">
+      <c r="A268" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="B268" s="6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="269" ht="15.75" customHeight="1">
+      <c r="A269" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B269" s="6" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="270" ht="15.75" customHeight="1">
+      <c r="A270" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="B270" s="6" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="271" ht="15.75" customHeight="1">
+      <c r="A271" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="B271" s="6" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="272" ht="15.75" customHeight="1">
+      <c r="A272" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="273" ht="15.75" customHeight="1">
+      <c r="A273" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="274" ht="15.75" customHeight="1">
+      <c r="A274" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B274" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="275" ht="15.75" customHeight="1">
+      <c r="A275" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="276" ht="15.75" customHeight="1">
+      <c r="A276" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="277" ht="15.75" customHeight="1">
+      <c r="A277" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="278" ht="15.75" customHeight="1">
+      <c r="A278" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="279" ht="15.75" customHeight="1">
+      <c r="A279" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="280" ht="15.75" customHeight="1">
+      <c r="A280" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="281" ht="15.75" customHeight="1">
+      <c r="A281" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="282" ht="15.75" customHeight="1">
+      <c r="A282" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="283" ht="15.75" customHeight="1">
+      <c r="A283" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="284" ht="15.75" customHeight="1">
+      <c r="A284" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="285" ht="15.75" customHeight="1">
+      <c r="A285" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="286" ht="15.75" customHeight="1">
+      <c r="A286" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="287" ht="15.75" customHeight="1">
+      <c r="A287" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="288" ht="15.75" customHeight="1">
+      <c r="A288" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="289" ht="15.75" customHeight="1">
+      <c r="A289" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="290" ht="15.75" customHeight="1">
+      <c r="A290" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="291" ht="15.75" customHeight="1">
+      <c r="A291" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="292" ht="15.75" customHeight="1">
+      <c r="A292" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="293" ht="15.75" customHeight="1">
+      <c r="A293" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="294" ht="15.75" customHeight="1">
+      <c r="A294" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="295" ht="15.75" customHeight="1">
+      <c r="A295" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="296" ht="15.75" customHeight="1">
+      <c r="A296" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="297" ht="15.75" customHeight="1">
+      <c r="A297" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="298" ht="15.75" customHeight="1">
+      <c r="A298" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="299" ht="15.75" customHeight="1">
+      <c r="A299" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="B299" s="6" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="300" ht="15.75" customHeight="1">
+      <c r="A300" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="B300" s="6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="301" ht="15.75" customHeight="1">
+      <c r="A301" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B301" s="6" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="302" ht="15.75" customHeight="1">
+      <c r="A302" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="B302" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="303" ht="15.75" customHeight="1">
+      <c r="A303" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="B303" s="6" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="304" ht="15.75" customHeight="1">
+      <c r="A304" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="305" ht="15.75" customHeight="1">
+      <c r="A305" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="306" ht="15.75" customHeight="1">
+      <c r="A306" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="B306" s="6" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="307" ht="15.75" customHeight="1">
+      <c r="A307" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="B307" s="6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="308" ht="15.75" customHeight="1">
+      <c r="A308" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="309" ht="15.75" customHeight="1">
+      <c r="A309" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="310" ht="15.75" customHeight="1">
+      <c r="A310" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="311" ht="15.75" customHeight="1">
+      <c r="A311" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="312" ht="15.75" customHeight="1">
+      <c r="A312" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="313" ht="15.75" customHeight="1">
+      <c r="A313" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="314" ht="15.75" customHeight="1">
+      <c r="A314" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="315" ht="15.75" customHeight="1">
+      <c r="A315" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="B315" s="6" t="s">
+        <v>628</v>
+      </c>
+    </row>
     <row r="316" ht="15.75" customHeight="1"/>
     <row r="317" ht="15.75" customHeight="1"/>
     <row r="318" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added logic to answer videos
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="677">
   <si>
     <t>Meme</t>
   </si>
@@ -1898,6 +1898,150 @@
   </si>
   <si>
     <t>CAACAgEAAxkBAAKsbGLQ3L2oCJo8QxbinGQEh8Bv9J6aAAL1AQACHCeJRnu9iot1Ezk3KQQ</t>
+  </si>
+  <si>
+    <t>veinte minutos despues | 20 minutos despues</t>
+  </si>
+  <si>
+    <t>video:20_minutos_despues.mp4 | time:20</t>
+  </si>
+  <si>
+    <t>346 minutos mas tarde</t>
+  </si>
+  <si>
+    <t>346_minutos_mas_tarde.mp4 time:346</t>
+  </si>
+  <si>
+    <t>una hora despues | 1 hora despues</t>
+  </si>
+  <si>
+    <t>video:1_hora_despues.mp4 | time:60</t>
+  </si>
+  <si>
+    <t>dos horas despues | 2 horas despues</t>
+  </si>
+  <si>
+    <t>video:2_horas_despues.mp4 | time:120</t>
+  </si>
+  <si>
+    <t>tres horas despues | 3 horas despues | tres horas despues puedes hacerlo de una vez</t>
+  </si>
+  <si>
+    <t>video:3_horas_despues_puedes_hacerlo_de_una_vez.mp4 | time:180</t>
+  </si>
+  <si>
+    <t>tres semanas despues | 3 semanas despues</t>
+  </si>
+  <si>
+    <t>video:3_semanas_despues.mp4 | time:30240</t>
+  </si>
+  <si>
+    <t>3 y 28 am | 3 y 28 de la madrugada | 3:28 am</t>
+  </si>
+  <si>
+    <t>video:3_y_28_de_la_madrugada.mp4</t>
+  </si>
+  <si>
+    <t>seis horas despues | 6 horas despues</t>
+  </si>
+  <si>
+    <t>video:6_horas_despues.mp4 | time:360</t>
+  </si>
+  <si>
+    <t>seis horas y media mas tarde | 6 horas y media mas tarde</t>
+  </si>
+  <si>
+    <t>video:6_hrs_y_media_mas_tarde.mp4 | time:390</t>
+  </si>
+  <si>
+    <t>8 pm y un minuto | 8:01 pm</t>
+  </si>
+  <si>
+    <t>video:8_pm_y_1_min.mp4</t>
+  </si>
+  <si>
+    <t>al dia siguiente</t>
+  </si>
+  <si>
+    <t>video:Al_dia_siguiente.mp4 | time:1440</t>
+  </si>
+  <si>
+    <t>media noche | 12 en punto media noche</t>
+  </si>
+  <si>
+    <t>12_en_punto_Media_noche.mp4</t>
+  </si>
+  <si>
+    <t>algunos centimetros mas tarde</t>
+  </si>
+  <si>
+    <t>video:Algunos_cm_mas_tarde.mp4</t>
+  </si>
+  <si>
+    <t>mañana</t>
+  </si>
+  <si>
+    <t>video:Mañana.mp4 | time:1440</t>
+  </si>
+  <si>
+    <t>mañana sin falta</t>
+  </si>
+  <si>
+    <t>video:Mañana_sin_falta.mp4 | time:1440</t>
+  </si>
+  <si>
+    <t>mientras tanto</t>
+  </si>
+  <si>
+    <t>Mientras_tanto.mp4</t>
+  </si>
+  <si>
+    <t>mucho mucho mas tarde</t>
+  </si>
+  <si>
+    <t>Mucho_mucho_mas_tarde.mp4</t>
+  </si>
+  <si>
+    <t>muchos meses despues</t>
+  </si>
+  <si>
+    <t>Muchos_Meses_Despues.mp4</t>
+  </si>
+  <si>
+    <t>nuevo narrador</t>
+  </si>
+  <si>
+    <t>Nuevo_Narrador.mp4</t>
+  </si>
+  <si>
+    <t>uhhhh</t>
+  </si>
+  <si>
+    <t>Uhhhh.mp4</t>
+  </si>
+  <si>
+    <t>una deuda con la sociedad mas tarde</t>
+  </si>
+  <si>
+    <t>Una_deuda_Con_la_sociedad_mas_tarde.mp4</t>
+  </si>
+  <si>
+    <t>unos momentos despues</t>
+  </si>
+  <si>
+    <t>Unos_momentos_despues.mp4</t>
+  </si>
+  <si>
+    <t>varias bromas malas despues</t>
+  </si>
+  <si>
+    <t>Varias_bromas_malas_despues.mp4</t>
+  </si>
+  <si>
+    <t>2000 años mas tarde</t>
+  </si>
+  <si>
+    <t>2000_años_más_tarde.mp4</t>
   </si>
 </sst>
 </file>
@@ -4712,30 +4856,198 @@
         <v>628</v>
       </c>
     </row>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1">
+      <c r="A316" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="317" ht="15.75" customHeight="1">
+      <c r="A317" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="318" ht="15.75" customHeight="1">
+      <c r="A318" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="B318" s="6" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="319" ht="15.75" customHeight="1">
+      <c r="A319" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="B319" s="6" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="320" ht="15.75" customHeight="1">
+      <c r="A320" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="321" ht="15.75" customHeight="1">
+      <c r="A321" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="322" ht="15.75" customHeight="1">
+      <c r="A322" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="B322" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="323" ht="15.75" customHeight="1">
+      <c r="A323" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="B323" s="6" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="324" ht="15.75" customHeight="1">
+      <c r="A324" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="B324" s="6" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="325" ht="15.75" customHeight="1">
+      <c r="A325" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="B325" s="6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="326" ht="15.75" customHeight="1">
+      <c r="A326" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="B326" s="6" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="327" ht="15.75" customHeight="1">
+      <c r="A327" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="B327" s="6" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="328" ht="15.75" customHeight="1">
+      <c r="A328" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="B328" s="6" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="329" ht="15.75" customHeight="1">
+      <c r="A329" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="330" ht="15.75" customHeight="1">
+      <c r="A330" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="B330" s="6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="331" ht="15.75" customHeight="1">
+      <c r="A331" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="332" ht="15.75" customHeight="1">
+      <c r="A332" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="333" ht="15.75" customHeight="1">
+      <c r="A333" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="334" ht="15.75" customHeight="1">
+      <c r="A334" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="335" ht="15.75" customHeight="1">
+      <c r="A335" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="B335" s="6" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="336" ht="15.75" customHeight="1">
+      <c r="A336" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="337" ht="15.75" customHeight="1">
+      <c r="A337" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="338" ht="15.75" customHeight="1">
+      <c r="A338" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="B339" s="6" t="s">
+        <v>676</v>
+      </c>
+    </row>
     <row r="340" ht="15.75" customHeight="1"/>
     <row r="341" ht="15.75" customHeight="1"/>
     <row r="342" ht="15.75" customHeight="1"/>
@@ -5388,6 +5700,9 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>

</xml_diff>

<commit_message>
Fixed logic to answer videos
Also some videos will repeat his answer after some time
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -1993,55 +1993,55 @@
     <t>mientras tanto</t>
   </si>
   <si>
-    <t>Mientras_tanto.mp4</t>
+    <t>video:Mientras_tanto.mp4</t>
   </si>
   <si>
     <t>mucho mucho mas tarde</t>
   </si>
   <si>
-    <t>Mucho_mucho_mas_tarde.mp4</t>
+    <t>video:Mucho_mucho_mas_tarde.mp4</t>
   </si>
   <si>
     <t>muchos meses despues</t>
   </si>
   <si>
-    <t>Muchos_Meses_Despues.mp4</t>
+    <t>video:Muchos_Meses_Despues.mp4</t>
   </si>
   <si>
     <t>nuevo narrador</t>
   </si>
   <si>
-    <t>Nuevo_Narrador.mp4</t>
+    <t>video:Nuevo_Narrador.mp4</t>
   </si>
   <si>
     <t>uhhhh</t>
   </si>
   <si>
-    <t>Uhhhh.mp4</t>
+    <t>video:Uhhhh.mp4</t>
   </si>
   <si>
     <t>una deuda con la sociedad mas tarde</t>
   </si>
   <si>
-    <t>Una_deuda_Con_la_sociedad_mas_tarde.mp4</t>
+    <t>video:Una_deuda_Con_la_sociedad_mas_tarde.mp4</t>
   </si>
   <si>
     <t>unos momentos despues</t>
   </si>
   <si>
-    <t>Unos_momentos_despues.mp4</t>
+    <t>video:Unos_momentos_despues.mp4</t>
   </si>
   <si>
     <t>varias bromas malas despues</t>
   </si>
   <si>
-    <t>Varias_bromas_malas_despues.mp4</t>
+    <t>video:Varias_bromas_malas_despues.mp4</t>
   </si>
   <si>
     <t>2000 años mas tarde</t>
   </si>
   <si>
-    <t>2000_años_más_tarde.mp4</t>
+    <t>video:2000_años_más_tarde.mp4</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Primera implementación de inline keyboard en versión 2.0
</commit_message>
<xml_diff>
--- a/data/meme_bot_db.xlsx
+++ b/data/meme_bot_db.xlsx
@@ -2374,10 +2374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B994"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B340" activeCellId="0" sqref="B340"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B319" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A341" activeCellId="0" sqref="A341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5758,7 +5758,7 @@
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>